<commit_message>
Running f1 and f2
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/F suite.xlsx
+++ b/src/test/resources/xls/F suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>TCID</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -613,10 +616,10 @@
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -630,7 +633,7 @@
         <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -644,7 +647,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new test case TestCase_F9 for notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/F suite.xlsx
+++ b/src/test/resources/xls/F suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>TCID</t>
   </si>
@@ -234,6 +234,15 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>TestCase_F9</t>
+  </si>
+  <si>
+    <t>OPQA-216</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following user comments on a post</t>
   </si>
 </sst>
 </file>
@@ -614,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -778,6 +787,23 @@
         <v>42</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new Test cases to Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/F suite.xlsx
+++ b/src/test/resources/xls/F suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>TCID</t>
   </si>
@@ -233,41 +233,58 @@
     <t>TestCase_F8</t>
   </si>
   <si>
+    <t>TestCase_F9</t>
+  </si>
+  <si>
+    <t>OPQA-216</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following user comments on a post</t>
+  </si>
+  <si>
+    <t>TestCase_F10</t>
+  </si>
+  <si>
+    <t>OPQA-217</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone comments on an post contained in his watchlist</t>
+  </si>
+  <si>
+    <t>TestCase_F11</t>
+  </si>
+  <si>
+    <t>OPQA-218</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification if someone likes his comment on a post</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>TestCase_F9</t>
-  </si>
-  <si>
-    <t>OPQA-216</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification when someone he is following user comments on a post</t>
-  </si>
-  <si>
-    <t>TestCase_F10</t>
-  </si>
-  <si>
-    <t>OPQA-217</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification when someone comments on an post contained in his watchlist</t>
-  </si>
-  <si>
-    <t>TestCase_F11</t>
-  </si>
-  <si>
-    <t>OPQA-218</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification if someone likes his comment on a post</t>
+    <t>TestCase_F12</t>
+  </si>
+  <si>
+    <t>OPQA-1183</t>
+  </si>
+  <si>
+    <t>Verify that user is receiving notification when someone he is following created a public watch list. (single event notification)</t>
+  </si>
+  <si>
+    <t>TestCase_F13</t>
+  </si>
+  <si>
+    <t>Verify that user is receiving notification when someone he is following made an existing watch list from private to public. (single event notification)</t>
+  </si>
+  <si>
+    <t>OPQA-1184</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -285,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +312,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,7 +351,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -342,7 +364,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,222 +667,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="105.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="135.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="3" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="3" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="3" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="7" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="7" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="7" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="7" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="3" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="B11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="3" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="B12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>46</v>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -876,108 +935,108 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="52.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="83.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="52.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="206.25" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="203.25" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="295.5" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="147" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="73.5" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="165.75" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="69.75" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Two Test Cases to Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/F suite.xlsx
+++ b/src/test/resources/xls/F suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
   <si>
     <t>TCID</t>
   </si>
@@ -297,6 +297,16 @@
   </si>
   <si>
     <t>Verify that users should be able to select from a list of suggested topics and check selected topic is presented in users type ahead</t>
+  </si>
+  <si>
+    <t>TestCase_F16</t>
+  </si>
+  <si>
+    <t>OPQA-231,OPQA-1100</t>
+  </si>
+  <si>
+    <t>Verify that Trending now section include articles and posts and able to navigate from tending now section and 
+Verify that Maximum count on the trending list is 10</t>
   </si>
 </sst>
 </file>
@@ -686,15 +696,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="135.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -969,6 +980,23 @@
         <v>42</v>
       </c>
       <c r="E16" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30">
+      <c r="A17" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding test cases for Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/F suite.xlsx
+++ b/src/test/resources/xls/F suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="97">
   <si>
     <t>TCID</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Verify that user receives a notification when someone he is following  publishes a post</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>TestCase_F6</t>
   </si>
   <si>
@@ -334,6 +331,27 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>TestCase_F20</t>
+  </si>
+  <si>
+    <t>OPQA-1011</t>
+  </si>
+  <si>
+    <t>Verify that follower of the post is able to start conversation from home page when some one commented on the post he is following.</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>Verify that author of the post is able to start conversation from home page when some one commented on his post.</t>
+  </si>
+  <si>
+    <t>TestCase_F21</t>
+  </si>
+  <si>
+    <t>OPQA-1010</t>
   </si>
 </sst>
 </file>
@@ -723,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,7 +787,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -786,7 +804,7 @@
         <v>42</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -794,16 +812,16 @@
         <v>32</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -820,7 +838,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -837,245 +855,279 @@
         <v>42</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="D7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="D10" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="D11" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="D12" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="D13" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D14" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="D16" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
       <c r="A17" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="D17" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="D18" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D19" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabling only two test cases in Notification Suite for testing
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/F suite.xlsx
+++ b/src/test/resources/xls/F suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
   <si>
     <t>TCID</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>OPQA-1010</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -818,7 +821,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>93</v>
@@ -835,7 +838,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>93</v>
@@ -852,7 +855,7 @@
         <v>45</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>93</v>
@@ -869,7 +872,7 @@
         <v>48</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>93</v>
@@ -886,7 +889,7 @@
         <v>52</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>93</v>
@@ -903,7 +906,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>93</v>
@@ -920,7 +923,7 @@
         <v>58</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>93</v>
@@ -937,7 +940,7 @@
         <v>61</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>93</v>
@@ -954,7 +957,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>93</v>
@@ -971,7 +974,7 @@
         <v>67</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>93</v>
@@ -988,7 +991,7 @@
         <v>69</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>93</v>
@@ -1005,7 +1008,7 @@
         <v>71</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>93</v>
@@ -1022,7 +1025,7 @@
         <v>76</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>93</v>
@@ -1039,7 +1042,7 @@
         <v>79</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>93</v>
@@ -1056,7 +1059,7 @@
         <v>82</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>93</v>
@@ -1073,7 +1076,7 @@
         <v>85</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>93</v>
@@ -1090,7 +1093,7 @@
         <v>86</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>93</v>
@@ -1107,7 +1110,7 @@
         <v>92</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>93</v>
@@ -1124,7 +1127,7 @@
         <v>94</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Configurations done for sanity suite to be run on prod
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/F suite.xlsx
+++ b/src/test/resources/xls/F suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="97">
   <si>
     <t>TCID</t>
   </si>
@@ -152,18 +152,6 @@
 2)Click on NOTES tab and verify that NOTES tab gets displayed with all the notes(if present).</t>
   </si>
   <si>
-    <t>TestCase_F1</t>
-  </si>
-  <si>
-    <t>TestCase_F2</t>
-  </si>
-  <si>
-    <t>TestCase_F3</t>
-  </si>
-  <si>
-    <t>TestCase_F4</t>
-  </si>
-  <si>
     <t>Verify that user receives a notification when he is followed by someone</t>
   </si>
   <si>
@@ -191,18 +179,12 @@
     <t>Y</t>
   </si>
   <si>
-    <t>TestCase_F5</t>
-  </si>
-  <si>
     <t>OPQA-877</t>
   </si>
   <si>
     <t>Verify that user receives a notification when someone he is following  publishes a post</t>
   </si>
   <si>
-    <t>TestCase_F6</t>
-  </si>
-  <si>
     <t>OPQA-213</t>
   </si>
   <si>
@@ -215,9 +197,6 @@
     <t>OPQA-210</t>
   </si>
   <si>
-    <t>TestCase_F7</t>
-  </si>
-  <si>
     <t>Verify that user receives a notification when someone comments on an article contained in his watchlist</t>
   </si>
   <si>
@@ -227,48 +206,30 @@
     <t>OPQA-215</t>
   </si>
   <si>
-    <t>TestCase_F8</t>
-  </si>
-  <si>
-    <t>TestCase_F9</t>
-  </si>
-  <si>
     <t>OPQA-216</t>
   </si>
   <si>
     <t>Verify that user receives a notification when someone he is following user comments on a post</t>
   </si>
   <si>
-    <t>TestCase_F10</t>
-  </si>
-  <si>
     <t>OPQA-217</t>
   </si>
   <si>
     <t>Verify that user receives a notification when someone comments on an post contained in his watchlist</t>
   </si>
   <si>
-    <t>TestCase_F11</t>
-  </si>
-  <si>
     <t>OPQA-218</t>
   </si>
   <si>
     <t>Verify that user receives a notification if someone likes his comment on a post</t>
   </si>
   <si>
-    <t>TestCase_F12</t>
-  </si>
-  <si>
     <t>OPQA-1183</t>
   </si>
   <si>
     <t>Verify that user is receiving notification when someone he is following created a public watch list. (single event notification)</t>
   </si>
   <si>
-    <t>TestCase_F13</t>
-  </si>
-  <si>
     <t>Verify that user is receiving notification when someone he is following made an existing watch list from private to public. (single event notification)</t>
   </si>
   <si>
@@ -278,22 +239,13 @@
     <t>Verify that user is receiving notification when someone liked his post(aggregated notification)</t>
   </si>
   <si>
-    <t>TestCase_F14</t>
-  </si>
-  <si>
     <t>OPQA-1013</t>
   </si>
   <si>
-    <t>TestCase_F15</t>
-  </si>
-  <si>
     <t>OPQA-226</t>
   </si>
   <si>
     <t>Verify that users should be able to select from a list of suggested topics and check selected topic is presented in users type ahead</t>
-  </si>
-  <si>
-    <t>TestCase_F16</t>
   </si>
   <si>
     <t>OPQA-231,OPQA-1100</t>
@@ -303,18 +255,12 @@
 Verify that Maximum count on the trending list is 10</t>
   </si>
   <si>
-    <t>TestCase_F17</t>
-  </si>
-  <si>
     <t>OPQA-1098</t>
   </si>
   <si>
     <t>Verify that Featured Post is at the top of event stream after login and that feature post should be top in post tab of trending section</t>
   </si>
   <si>
-    <t>TestCase_F18</t>
-  </si>
-  <si>
     <t>OPQA-1099</t>
   </si>
   <si>
@@ -327,15 +273,9 @@
     <t>OPQA-1012</t>
   </si>
   <si>
-    <t>TestCase_F19</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>TestCase_F20</t>
-  </si>
-  <si>
     <t>OPQA-1011</t>
   </si>
   <si>
@@ -348,13 +288,70 @@
     <t>Verify that author of the post is able to start conversation from home page when some one commented on his post.</t>
   </si>
   <si>
-    <t>TestCase_F21</t>
-  </si>
-  <si>
     <t>OPQA-1010</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Notifications001</t>
+  </si>
+  <si>
+    <t>Notifications002</t>
+  </si>
+  <si>
+    <t>Notifications003</t>
+  </si>
+  <si>
+    <t>Notifications004</t>
+  </si>
+  <si>
+    <t>Notifications005</t>
+  </si>
+  <si>
+    <t>Notifications006</t>
+  </si>
+  <si>
+    <t>Notifications007</t>
+  </si>
+  <si>
+    <t>Notifications008</t>
+  </si>
+  <si>
+    <t>Notifications009</t>
+  </si>
+  <si>
+    <t>Notifications010</t>
+  </si>
+  <si>
+    <t>Notifications011</t>
+  </si>
+  <si>
+    <t>Notifications012</t>
+  </si>
+  <si>
+    <t>Notifications013</t>
+  </si>
+  <si>
+    <t>Notifications014</t>
+  </si>
+  <si>
+    <t>Notifications015</t>
+  </si>
+  <si>
+    <t>Notifications016</t>
+  </si>
+  <si>
+    <t>Notifications017</t>
+  </si>
+  <si>
+    <t>Notifications018</t>
+  </si>
+  <si>
+    <t>Notifications019</t>
+  </si>
+  <si>
+    <t>Notifications020</t>
+  </si>
+  <si>
+    <t>Notifications021</t>
   </si>
 </sst>
 </file>
@@ -746,13 +743,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="135.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
@@ -764,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -778,359 +775,359 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
       <c r="A17" s="6" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>